<commit_message>
Mejora de Sucursal, se incluye horarioLaboral
</commit_message>
<xml_diff>
--- a/SpaOnline/Sucursales - Muestreo Datos.xlsx
+++ b/SpaOnline/Sucursales - Muestreo Datos.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE5CCD8-DDF5-4A33-B1D8-981D45CB2ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{CFE5CCD8-DDF5-4A33-B1D8-981D45CB2ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E38FC89-3272-40C8-9287-48E8BEC6C524}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Sucursal" sheetId="5" r:id="rId3"/>
-    <sheet name="Pais" sheetId="6" r:id="rId4"/>
-    <sheet name="Departamento" sheetId="7" r:id="rId5"/>
-    <sheet name="Ciudad" sheetId="8" r:id="rId6"/>
-    <sheet name="TipoIdentificacion" sheetId="9" r:id="rId7"/>
+    <sheet name="HorarioLaboral" sheetId="10" r:id="rId4"/>
+    <sheet name="Pais" sheetId="6" r:id="rId5"/>
+    <sheet name="Departamento" sheetId="7" r:id="rId6"/>
+    <sheet name="Ciudad" sheetId="8" r:id="rId7"/>
+    <sheet name="TipoIdentificacion" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -200,13 +201,34 @@
   </si>
   <si>
     <t>SucursalPoblado@gmail.com</t>
+  </si>
+  <si>
+    <t>HoraInicio</t>
+  </si>
+  <si>
+    <t>HoraFin</t>
+  </si>
+  <si>
+    <t>8:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>6:00</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>HorarioLaboral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +248,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -286,12 +314,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -324,6 +361,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -744,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,15 +907,16 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -885,25 +927,28 @@
         <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -914,29 +959,33 @@
       <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="13" t="str">
+      <c r="D2" s="18" t="str">
+        <f>HorarioLaboral!D2</f>
+        <v>8:00-19:00</v>
+      </c>
+      <c r="E2" s="13" t="str">
         <f>Ciudad!E2</f>
         <v>Rionegro-Antioquia-Colombia</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>54323243</v>
       </c>
-      <c r="H2" s="5" t="str">
-        <f>B2&amp;"-"&amp;D2&amp;"-"&amp;E2</f>
+      <c r="I2" s="5" t="str">
+        <f>B2&amp;"-"&amp;E2&amp;"-"&amp;F2</f>
         <v>NIT-Rionegro-Antioquia-Colombia-CL 10 43 A 29</v>
       </c>
-      <c r="I2" s="16" t="str">
-        <f>F2&amp;"-"&amp;G2</f>
+      <c r="J2" s="16" t="str">
+        <f>G2&amp;"-"&amp;H2</f>
         <v>SucursalRionegro@gmail.com-54323243</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -947,29 +996,33 @@
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="13" t="str">
+      <c r="D3" s="18" t="str">
+        <f>HorarioLaboral!D3</f>
+        <v>6:00-17:00</v>
+      </c>
+      <c r="E3" s="13" t="str">
         <f>Ciudad!E3</f>
         <v>Marinilla-Antioquia-Colombia</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>3214321</v>
       </c>
-      <c r="H3" s="5" t="str">
-        <f t="shared" ref="H3:I4" si="0">B3&amp;"-"&amp;D3&amp;"-"&amp;E3</f>
+      <c r="I3" s="5" t="str">
+        <f t="shared" ref="I3:I4" si="0">B3&amp;"-"&amp;E3&amp;"-"&amp;F3</f>
         <v>NIT-Marinilla-Antioquia-Colombia-CL 63 9 36</v>
       </c>
-      <c r="I3" s="16" t="str">
-        <f t="shared" ref="I3:I4" si="1">F3&amp;"-"&amp;G3</f>
+      <c r="J3" s="16" t="str">
+        <f t="shared" ref="J3:J4" si="1">G3&amp;"-"&amp;H3</f>
         <v>SucursalMarinilla@gmail.com-3214321</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -980,48 +1033,116 @@
       <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="13" t="str">
+      <c r="D4" s="18" t="str">
+        <f>HorarioLaboral!D2</f>
+        <v>8:00-19:00</v>
+      </c>
+      <c r="E4" s="13" t="str">
         <f>Ciudad!E4</f>
         <v>Medellin-Antioquia-Colombia</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>5632421</v>
       </c>
-      <c r="H4" s="5" t="str">
+      <c r="I4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>NIT-Medellin-Antioquia-Colombia-CR 2 5 39</v>
       </c>
-      <c r="I4" s="16" t="str">
+      <c r="J4" s="16" t="str">
         <f t="shared" si="1"/>
         <v>SucursalPoblado@gmail.com-5632421</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="10"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" location="TipoIdentificacion!C4" display="TipoIdentificacion!C4" xr:uid="{99331531-149B-4697-B677-7BF6638CAEC8}"/>
     <hyperlink ref="B3" location="TipoIdentificacion!C4" display="TipoIdentificacion!C4" xr:uid="{592A1D9F-4248-4D41-8C28-54D5FA6576C8}"/>
     <hyperlink ref="B4" location="TipoIdentificacion!C4" display="TipoIdentificacion!C4" xr:uid="{0A2CF45A-6E62-46DB-8001-4511A6F6E666}"/>
-    <hyperlink ref="D2" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{2B6EFE98-886D-482A-B20E-687296015F04}"/>
-    <hyperlink ref="D3:D4" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{BC45D5CC-AD1A-4653-96DD-CDBDC908237C}"/>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{0663BB21-9A43-4B1D-8A21-551F857989D3}"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="SucursalRionegr@gmail.com" xr:uid="{F9F2D69F-AEA3-489F-9DFD-69BF6E19218A}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{5F355592-918F-4243-92D4-800C7FC291AF}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{A86DA135-0247-4A09-A184-77E7675764A2}"/>
+    <hyperlink ref="E2" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{2B6EFE98-886D-482A-B20E-687296015F04}"/>
+    <hyperlink ref="E3:E4" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{BC45D5CC-AD1A-4653-96DD-CDBDC908237C}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{0663BB21-9A43-4B1D-8A21-551F857989D3}"/>
+    <hyperlink ref="G3:G4" r:id="rId2" display="SucursalRionegr@gmail.com" xr:uid="{F9F2D69F-AEA3-489F-9DFD-69BF6E19218A}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{5F355592-918F-4243-92D4-800C7FC291AF}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{A86DA135-0247-4A09-A184-77E7675764A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5576EA1-41AD-4B56-A015-05E993B07C02}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f>B2&amp;"-"&amp;C2</f>
+        <v>8:00-19:00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f>B3&amp;"-"&amp;C3</f>
+        <v>6:00-17:00</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8CC05-D5A5-4217-82D6-119F47E099F6}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1086,7 +1207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A945E5-5B27-42C4-B638-F59EC3627386}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1173,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91524816-6EF0-4C72-9C90-F3A24E79B63C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1288,7 +1409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD8BDB0-B92E-403D-81E8-218137D380CF}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>